<commit_message>
Restructured the code to work with John's latest piece of VBA for positioning and cashflows.
</commit_message>
<xml_diff>
--- a/Rebalancing/assets/Risk Rated Targets Updated 15 05 2023.xlsx
+++ b/Rebalancing/assets/Risk Rated Targets Updated 15 05 2023.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Fund Management\Fund Management Team Files\FM Personal Folders\Richard\PycharmProjects\Rebalancing\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FCCF76-0470-44D2-8C89-FC8849B53072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE211A98-C51C-4224-8F6D-F3DA56CFC8E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33870" yWindow="-18915" windowWidth="7590" windowHeight="3405" activeTab="2" xr2:uid="{1B5CF6ED-69C4-4295-ADBC-52871FB68B92}"/>
+    <workbookView xWindow="-1965" yWindow="-21885" windowWidth="7590" windowHeight="3405" activeTab="3" xr2:uid="{1B5CF6ED-69C4-4295-ADBC-52871FB68B92}"/>
   </bookViews>
   <sheets>
-    <sheet name="Providence Targets" sheetId="2" r:id="rId1"/>
-    <sheet name="Select Targets" sheetId="3" r:id="rId2"/>
-    <sheet name="International Targets" sheetId="4" r:id="rId3"/>
-    <sheet name="Venture Targets" sheetId="1" r:id="rId4"/>
+    <sheet name="Providence" sheetId="2" r:id="rId1"/>
+    <sheet name="Select" sheetId="3" r:id="rId2"/>
+    <sheet name="International" sheetId="4" r:id="rId3"/>
+    <sheet name="Venture" sheetId="1" r:id="rId4"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId5"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="175">
   <si>
     <t>SEDOL</t>
   </si>
@@ -549,6 +549,24 @@
   </si>
   <si>
     <t>0580353</t>
+  </si>
+  <si>
+    <t>Providence</t>
+  </si>
+  <si>
+    <t>392125</t>
+  </si>
+  <si>
+    <t>392126</t>
+  </si>
+  <si>
+    <t>Select</t>
+  </si>
+  <si>
+    <t>392124</t>
+  </si>
+  <si>
+    <t>International</t>
   </si>
 </sst>
 </file>
@@ -970,12 +988,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1012,6 +1024,12 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2327,6 +2345,14 @@
           </cell>
           <cell r="B156" t="str">
             <v>CIS</v>
+          </cell>
+        </row>
+        <row r="157">
+          <cell r="A157" t="str">
+            <v>0643610</v>
+          </cell>
+          <cell r="B157" t="str">
+            <v>Broker</v>
           </cell>
         </row>
         <row r="222">
@@ -2768,10 +2794,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BA10D10-D38A-48DE-9203-9D84F968A0CA}">
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:I16"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2824,11 +2850,11 @@
       <c r="K1" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="M1" s="45"/>
-      <c r="N1" s="46"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="62"/>
     </row>
     <row r="2" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -2862,10 +2888,10 @@
         <v>CIS</v>
       </c>
       <c r="J2" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="K2" s="26">
-        <v>392128</v>
+        <v>169</v>
+      </c>
+      <c r="K2" s="26" t="s">
+        <v>170</v>
       </c>
       <c r="L2" s="36" t="s">
         <v>72</v>
@@ -2876,7 +2902,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="48" t="s">
         <v>95</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -2916,7 +2942,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="48" t="s">
         <v>96</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -2954,7 +2980,7 @@
       <c r="N4" s="44"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="47" t="s">
         <v>97</v>
       </c>
       <c r="B5" s="34" t="s">
@@ -2987,7 +3013,7 @@
       <c r="J5" s="22"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="48" t="s">
         <v>98</v>
       </c>
       <c r="B6" s="9" t="s">
@@ -3020,7 +3046,7 @@
       <c r="J6" s="22"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="50" t="s">
+      <c r="A7" s="48" t="s">
         <v>99</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -3053,7 +3079,7 @@
       <c r="J7" s="22"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="50" t="s">
+      <c r="A8" s="48" t="s">
         <v>44</v>
       </c>
       <c r="B8" s="9" t="s">
@@ -3086,7 +3112,7 @@
       <c r="J8" s="22"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="49" t="s">
+      <c r="A9" s="47" t="s">
         <v>100</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -3119,7 +3145,7 @@
       <c r="J9" s="22"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="48" t="s">
         <v>101</v>
       </c>
       <c r="B10" s="9" t="s">
@@ -3152,7 +3178,7 @@
       <c r="J10" s="22"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="50" t="s">
+      <c r="A11" s="48" t="s">
         <v>102</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -3185,7 +3211,7 @@
       <c r="J11" s="22"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="50" t="s">
+      <c r="A12" s="48" t="s">
         <v>103</v>
       </c>
       <c r="B12" s="9" t="s">
@@ -3218,7 +3244,7 @@
       <c r="J12" s="22"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="50" t="s">
+      <c r="A13" s="48" t="s">
         <v>104</v>
       </c>
       <c r="B13" s="9" t="s">
@@ -3251,7 +3277,7 @@
       <c r="J13" s="22"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="49" t="s">
+      <c r="A14" s="47" t="s">
         <v>105</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -3284,7 +3310,7 @@
       <c r="J14" s="22"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="50" t="s">
+      <c r="A15" s="48" t="s">
         <v>106</v>
       </c>
       <c r="B15" s="9" t="s">
@@ -3317,7 +3343,7 @@
       <c r="J15" s="22"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="50" t="s">
+      <c r="A16" s="48" t="s">
         <v>107</v>
       </c>
       <c r="B16" s="9" t="s">
@@ -3389,146 +3415,11 @@
       </c>
       <c r="G19" s="4"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>81</v>
-      </c>
-      <c r="C22" t="b">
-        <f>IF(B22=B2, TRUE, FALSE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>82</v>
-      </c>
-      <c r="C23" t="b">
-        <f t="shared" ref="C23:C36" si="2">IF(B23=B3, TRUE, FALSE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>83</v>
-      </c>
-      <c r="C24" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>84</v>
-      </c>
-      <c r="C25" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>85</v>
-      </c>
-      <c r="C26" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>86</v>
-      </c>
-      <c r="C27" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>87</v>
-      </c>
-      <c r="C29" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>88</v>
-      </c>
-      <c r="C30" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>89</v>
-      </c>
-      <c r="C31" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>90</v>
-      </c>
-      <c r="C32" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>91</v>
-      </c>
-      <c r="C33" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>92</v>
-      </c>
-      <c r="C34" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>93</v>
-      </c>
-      <c r="C35" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>94</v>
-      </c>
-      <c r="C36" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="L1:N1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A2:I21 A38:I94 E22:I37 A22:C37">
+  <conditionalFormatting sqref="A2:I78">
     <cfRule type="expression" dxfId="3" priority="1">
       <formula>$G2&lt;&gt;0</formula>
     </cfRule>
@@ -3541,18 +3432,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{098E9D01-23BA-4243-973E-F49402050783}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" style="53" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="51" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="70.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="61" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="59" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" style="59" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
@@ -3562,7 +3453,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="29" t="s">
@@ -3574,10 +3465,10 @@
       <c r="D1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="55" t="s">
+      <c r="E1" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="56" t="s">
+      <c r="F1" s="54" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="31" t="s">
@@ -3595,11 +3486,11 @@
       <c r="K1" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="M1" s="45"/>
-      <c r="N1" s="46"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="62"/>
     </row>
     <row r="2" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -3615,10 +3506,10 @@
       <c r="D2" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="E2" s="57">
+      <c r="E2" s="55">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="F2" s="57">
+      <c r="F2" s="55">
         <v>0.04</v>
       </c>
       <c r="G2" s="4">
@@ -3633,10 +3524,10 @@
         <v>CIS</v>
       </c>
       <c r="J2" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="K2" s="26">
-        <v>392128</v>
+        <v>172</v>
+      </c>
+      <c r="K2" s="26" t="s">
+        <v>171</v>
       </c>
       <c r="L2" s="36" t="s">
         <v>72</v>
@@ -3647,7 +3538,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="45" t="s">
         <v>136</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -3660,10 +3551,10 @@
       <c r="D3" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="E3" s="58">
+      <c r="E3" s="56">
         <v>0.03</v>
       </c>
-      <c r="F3" s="58">
+      <c r="F3" s="56">
         <v>0.03</v>
       </c>
       <c r="G3" s="4">
@@ -3687,7 +3578,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="45" t="s">
         <v>137</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -3700,10 +3591,10 @@
       <c r="D4" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="E4" s="58">
+      <c r="E4" s="56">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="F4" s="58">
+      <c r="F4" s="56">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="G4" s="4">
@@ -3738,10 +3629,10 @@
       <c r="D5" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="E5" s="58">
+      <c r="E5" s="56">
         <v>0.05</v>
       </c>
-      <c r="F5" s="58">
+      <c r="F5" s="56">
         <v>0.05</v>
       </c>
       <c r="G5" s="4">
@@ -3758,7 +3649,7 @@
       <c r="J5" s="22"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="45" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="9" t="s">
@@ -3771,10 +3662,10 @@
       <c r="D6" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="58">
+      <c r="E6" s="56">
         <v>5.7500000000000002E-2</v>
       </c>
-      <c r="F6" s="58">
+      <c r="F6" s="56">
         <v>5.7500000000000002E-2</v>
       </c>
       <c r="G6" s="4">
@@ -3791,7 +3682,7 @@
       <c r="J6" s="22"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="45" t="s">
         <v>139</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -3804,10 +3695,10 @@
       <c r="D7" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="E7" s="58">
+      <c r="E7" s="56">
         <v>7.2499999999999995E-2</v>
       </c>
-      <c r="F7" s="58">
+      <c r="F7" s="56">
         <v>0.1075</v>
       </c>
       <c r="G7" s="4">
@@ -3824,7 +3715,7 @@
       <c r="J7" s="22"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="45" t="s">
         <v>38</v>
       </c>
       <c r="B8" s="9" t="s">
@@ -3837,10 +3728,10 @@
       <c r="D8" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="58">
+      <c r="E8" s="56">
         <v>0.06</v>
       </c>
-      <c r="F8" s="58">
+      <c r="F8" s="56">
         <v>0.06</v>
       </c>
       <c r="G8" s="4">
@@ -3870,10 +3761,10 @@
       <c r="D9" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E9" s="59">
+      <c r="E9" s="57">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="F9" s="59">
+      <c r="F9" s="57">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="G9" s="4">
@@ -3890,7 +3781,7 @@
       <c r="J9" s="22"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="45" t="s">
         <v>44</v>
       </c>
       <c r="B10" s="9" t="s">
@@ -3903,10 +3794,10 @@
       <c r="D10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="58">
+      <c r="E10" s="56">
         <v>0.06</v>
       </c>
-      <c r="F10" s="58">
+      <c r="F10" s="56">
         <v>0.06</v>
       </c>
       <c r="G10" s="4">
@@ -3923,7 +3814,7 @@
       <c r="J10" s="22"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="45" t="s">
         <v>141</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -3936,10 +3827,10 @@
       <c r="D11" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="E11" s="58">
+      <c r="E11" s="56">
         <v>7.2499999999999995E-2</v>
       </c>
-      <c r="F11" s="58">
+      <c r="F11" s="56">
         <v>7.2499999999999995E-2</v>
       </c>
       <c r="G11" s="4">
@@ -3956,7 +3847,7 @@
       <c r="J11" s="22"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="45" t="s">
         <v>142</v>
       </c>
       <c r="B12" s="9" t="s">
@@ -3969,10 +3860,10 @@
       <c r="D12" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="E12" s="58">
+      <c r="E12" s="56">
         <v>0.05</v>
       </c>
-      <c r="F12" s="58">
+      <c r="F12" s="56">
         <v>0.05</v>
       </c>
       <c r="G12" s="4">
@@ -3989,7 +3880,7 @@
       <c r="J12" s="22"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="45" t="s">
         <v>102</v>
       </c>
       <c r="B13" s="9" t="s">
@@ -4002,10 +3893,10 @@
       <c r="D13" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="E13" s="58">
+      <c r="E13" s="56">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="F13" s="58">
+      <c r="F13" s="56">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="G13" s="4">
@@ -4035,10 +3926,10 @@
       <c r="D14" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E14" s="59">
+      <c r="E14" s="57">
         <v>0.09</v>
       </c>
-      <c r="F14" s="59">
+      <c r="F14" s="57">
         <v>0.09</v>
       </c>
       <c r="G14" s="4">
@@ -4055,7 +3946,7 @@
       <c r="J14" s="22"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="47" t="s">
+      <c r="A15" s="45" t="s">
         <v>104</v>
       </c>
       <c r="B15" s="9" t="s">
@@ -4068,10 +3959,10 @@
       <c r="D15" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="E15" s="58">
+      <c r="E15" s="56">
         <v>0.02</v>
       </c>
-      <c r="F15" s="58">
+      <c r="F15" s="56">
         <v>0.02</v>
       </c>
       <c r="G15" s="4">
@@ -4088,7 +3979,7 @@
       <c r="J15" s="22"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="45" t="s">
         <v>105</v>
       </c>
       <c r="B16" s="9" t="s">
@@ -4101,10 +3992,10 @@
       <c r="D16" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E16" s="59">
+      <c r="E16" s="57">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="F16" s="59">
+      <c r="F16" s="57">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="G16" s="4">
@@ -4121,7 +4012,7 @@
       <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="46" t="s">
         <v>143</v>
       </c>
       <c r="B17" s="35" t="s">
@@ -4134,10 +4025,10 @@
       <c r="D17" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E17" s="57">
+      <c r="E17" s="55">
         <v>0.03</v>
       </c>
-      <c r="F17" s="57">
+      <c r="F17" s="55">
         <v>0.03</v>
       </c>
       <c r="G17" s="4">
@@ -4154,7 +4045,7 @@
       <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="47" t="s">
+      <c r="A18" s="45" t="s">
         <v>144</v>
       </c>
       <c r="B18" s="9" t="s">
@@ -4167,10 +4058,10 @@
       <c r="D18" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="E18" s="58">
+      <c r="E18" s="56">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="F18" s="58">
+      <c r="F18" s="56">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="G18" s="4">
@@ -4190,24 +4081,24 @@
       <c r="B19" s="12"/>
       <c r="C19" s="2"/>
       <c r="D19" s="12"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="59"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
       <c r="G19" s="4"/>
       <c r="H19" s="14"/>
       <c r="I19" s="5"/>
       <c r="J19" s="22"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="54"/>
+      <c r="A20" s="52"/>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
       <c r="D20" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="60">
+      <c r="E20" s="58">
         <v>1.7500000000000002E-2</v>
       </c>
-      <c r="F20" s="62">
+      <c r="F20" s="60">
         <v>1.7500000000000002E-2</v>
       </c>
       <c r="G20" s="4"/>
@@ -4216,11 +4107,11 @@
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21" s="20"/>
       <c r="C21" s="17"/>
-      <c r="E21" s="61">
+      <c r="E21" s="59">
         <f>SUM(E2:E20)</f>
         <v>0.99999999999999989</v>
       </c>
-      <c r="F21" s="57">
+      <c r="F21" s="55">
         <f>SUM(F2:F20)</f>
         <v>0.99999999999999989</v>
       </c>
@@ -4244,13 +4135,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A1E2D3F-50F2-424D-8072-3D8544AD7059}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:I18"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" style="53" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="51" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="70.42578125" bestFit="1" customWidth="1"/>
@@ -4265,7 +4156,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="29" t="s">
@@ -4298,11 +4189,11 @@
       <c r="K1" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="M1" s="45"/>
-      <c r="N1" s="46"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="62"/>
     </row>
     <row r="2" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -4336,10 +4227,10 @@
         <v>CIS</v>
       </c>
       <c r="J2" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="K2" s="26">
-        <v>392128</v>
+        <v>174</v>
+      </c>
+      <c r="K2" s="26" t="s">
+        <v>173</v>
       </c>
       <c r="L2" s="36" t="s">
         <v>72</v>
@@ -4350,7 +4241,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="45" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -4390,7 +4281,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="45" t="s">
         <v>136</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -4461,7 +4352,7 @@
       <c r="J5" s="22"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="45" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="9" t="s">
@@ -4494,7 +4385,7 @@
       <c r="J6" s="22"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="45" t="s">
         <v>138</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -4527,7 +4418,7 @@
       <c r="J7" s="22"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="45" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="9" t="s">
@@ -4593,7 +4484,7 @@
       <c r="J9" s="22"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="45" t="s">
         <v>165</v>
       </c>
       <c r="B10" s="9" t="s">
@@ -4626,7 +4517,7 @@
       <c r="J10" s="22"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="45" t="s">
         <v>44</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -4659,7 +4550,7 @@
       <c r="J11" s="22"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="45" t="s">
         <v>47</v>
       </c>
       <c r="B12" s="9" t="s">
@@ -4692,7 +4583,7 @@
       <c r="J12" s="22"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="45" t="s">
         <v>142</v>
       </c>
       <c r="B13" s="9" t="s">
@@ -4758,7 +4649,7 @@
       <c r="J14" s="22"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="47" t="s">
+      <c r="A15" s="45" t="s">
         <v>166</v>
       </c>
       <c r="B15" s="9" t="s">
@@ -4791,7 +4682,7 @@
       <c r="J15" s="22"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="45" t="s">
         <v>60</v>
       </c>
       <c r="B16" s="9" t="s">
@@ -4824,7 +4715,7 @@
       <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="46" t="s">
         <v>66</v>
       </c>
       <c r="B17" s="35" t="s">
@@ -4857,7 +4748,7 @@
       <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="47" t="s">
+      <c r="A18" s="45" t="s">
         <v>167</v>
       </c>
       <c r="B18" s="9" t="s">
@@ -4901,7 +4792,7 @@
       <c r="J19" s="22"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="54"/>
+      <c r="A20" s="52"/>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
       <c r="D20" s="16" t="s">
@@ -4946,7 +4837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AECF6E9F-7227-4193-A8E8-8AAEBCC44F58}">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4998,14 +4889,14 @@
       <c r="K1" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="M1" s="45"/>
-      <c r="N1" s="46"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="62"/>
     </row>
     <row r="2" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="47" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -5050,7 +4941,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="48" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -5090,7 +4981,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="48" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -5128,7 +5019,7 @@
       <c r="N4" s="44"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="47" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="34" t="s">
@@ -5161,7 +5052,7 @@
       <c r="J5" s="22"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="48" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="9" t="s">
@@ -5194,7 +5085,7 @@
       <c r="J6" s="22"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="50" t="s">
+      <c r="A7" s="48" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -5227,7 +5118,7 @@
       <c r="J7" s="22"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="50" t="s">
+      <c r="A8" s="48" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="9" t="s">
@@ -5260,7 +5151,7 @@
       <c r="J8" s="22"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="49" t="s">
+      <c r="A9" s="47" t="s">
         <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -5293,7 +5184,7 @@
       <c r="J9" s="22"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="48" t="s">
         <v>35</v>
       </c>
       <c r="B10" s="9" t="s">
@@ -5326,7 +5217,7 @@
       <c r="J10" s="22"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="50" t="s">
+      <c r="A11" s="48" t="s">
         <v>38</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -5359,7 +5250,7 @@
       <c r="J11" s="22"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="50" t="s">
+      <c r="A12" s="48" t="s">
         <v>41</v>
       </c>
       <c r="B12" s="9" t="s">
@@ -5392,7 +5283,7 @@
       <c r="J12" s="22"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="50" t="s">
+      <c r="A13" s="48" t="s">
         <v>44</v>
       </c>
       <c r="B13" s="9" t="s">
@@ -5425,7 +5316,7 @@
       <c r="J13" s="22"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="49" t="s">
+      <c r="A14" s="47" t="s">
         <v>47</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -5458,7 +5349,7 @@
       <c r="J14" s="22"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="50" t="s">
+      <c r="A15" s="48" t="s">
         <v>50</v>
       </c>
       <c r="B15" s="9" t="s">
@@ -5491,7 +5382,7 @@
       <c r="J15" s="22"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="50" t="s">
+      <c r="A16" s="48" t="s">
         <v>53</v>
       </c>
       <c r="B16" s="9" t="s">
@@ -5524,7 +5415,7 @@
       <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="51" t="s">
+      <c r="A17" s="49" t="s">
         <v>56</v>
       </c>
       <c r="B17" s="35" t="s">
@@ -5557,7 +5448,7 @@
       <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="50" t="s">
+      <c r="A18" s="48" t="s">
         <v>60</v>
       </c>
       <c r="B18" s="9" t="s">
@@ -5590,7 +5481,7 @@
       <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="50" t="s">
+      <c r="A19" s="48" t="s">
         <v>63</v>
       </c>
       <c r="B19" s="9" t="s">
@@ -5623,7 +5514,7 @@
       <c r="J19" s="22"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="49" t="s">
+      <c r="A20" s="47" t="s">
         <v>66</v>
       </c>
       <c r="B20" s="1" t="s">

</xml_diff>